<commit_message>
ran code and data
</commit_message>
<xml_diff>
--- a/data/2021-08-30_shewy_layout.xlsx
+++ b/data/2021-08-30_shewy_layout.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pate212/GitHub/stillage_general_script/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garc286/RStudio/stillage_general_script/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AA1C7F-8F93-D549-87BA-BEEBE2D1AEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F9A8D5-B51D-4844-BED1-3E1BCDB81E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38380" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{318F1633-56B8-984D-8E8D-FBAE4BE2DA50}"/>
+    <workbookView xWindow="3660" yWindow="1440" windowWidth="28800" windowHeight="18000" xr2:uid="{318F1633-56B8-984D-8E8D-FBAE4BE2DA50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="notes" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="47">
   <si>
     <t>96 well plate template</t>
   </si>
@@ -154,10 +154,28 @@
     <t>Well</t>
   </si>
   <si>
-    <t>O2 limit_Blk</t>
-  </si>
-  <si>
-    <t>Fodder yeat_Blk</t>
+    <t xml:space="preserve"> Anaerobic lacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anaerobic lacto_Blk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aerobic lacto</t>
+  </si>
+  <si>
+    <t>O2 limit lacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aerobic lacto_Blk</t>
+  </si>
+  <si>
+    <t>O2 limit lacto_Blk</t>
+  </si>
+  <si>
+    <t>Fodder yeast</t>
+  </si>
+  <si>
+    <t>Fodder yeast_Blk</t>
   </si>
 </sst>
 </file>
@@ -759,7 +777,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,22 +837,22 @@
         <v>22</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>13</v>
+      <c r="I2" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="J2" s="30" t="s">
         <v>32</v>
@@ -860,22 +878,22 @@
         <v>22</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="32" t="s">
-        <v>13</v>
+      <c r="I3" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J3" s="33" t="s">
         <v>32</v>
@@ -901,22 +919,22 @@
         <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H4" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="32" t="s">
-        <v>13</v>
+      <c r="I4" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J4" s="33" t="s">
         <v>32</v>
@@ -942,22 +960,22 @@
         <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="32" t="s">
-        <v>13</v>
+      <c r="I5" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J5" s="33" t="s">
         <v>32</v>
@@ -983,22 +1001,22 @@
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H6" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="32" t="s">
-        <v>33</v>
+      <c r="I6" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>32</v>
@@ -1024,22 +1042,22 @@
         <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>33</v>
+      <c r="I7" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>32</v>
@@ -1065,22 +1083,22 @@
         <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>33</v>
+      <c r="I8" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>32</v>
@@ -1106,22 +1124,22 @@
         <v>23</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H9" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>33</v>
+      <c r="I9" s="36" t="s">
+        <v>32</v>
       </c>
       <c r="J9" s="36" t="s">
         <v>32</v>

</xml_diff>